<commit_message>
(Committed the questionnaire because I want to switch branches, but I don't think anything changed)
</commit_message>
<xml_diff>
--- a/data/EU-EpiCap_Questionnaire_21_11_30.xlsx
+++ b/data/EU-EpiCap_Questionnaire_21_11_30.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://surreyac-my.sharepoint.com/personal/cb0078_surrey_ac_uk/Documents/MATRIX/WP4-T2/EU-EpiCap-Tool/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{B2ED66EE-9066-4F67-9A9C-C5FF33F2DB6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8DA975F2-D9F9-4887-976F-B8773A25E1B0}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{45270A84-C129-4EA0-9102-B014D4D5961B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{28526098-AC66-4E22-BDF6-508079EF737A}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="1050" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="5" r:id="rId1"/>
@@ -186,13 +186,6 @@
     <t>Would you consider that the objective of the OH surveillance system has been defined from the expectations of all stakeholders including surveillance actors and end-users?</t>
   </si>
   <si>
-    <t xml:space="preserve">1. No cross-sectoral objective was defined.
-2. A cross-sectoral objective for the OH surveillance system was defined but is not based on stakeholders’ expectations.
-3. A cross-sectoral objective for the OH surveillance system was defined based on some stakeholders’ expectations.
-4. A cross-sectoral objective for the OH surveillance system was defined based on all stakeholders’ expectations.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. There is no supporting documentation.
 2. There are support documents but only parts of the items are mentioned.
 3. The support documents include all items but are not shared with all actors.
@@ -1119,6 +1112,12 @@
   </si>
   <si>
     <t>Target 3.4 Ultimate outcomes</t>
+  </si>
+  <si>
+    <t>1. No cross-sectoral objective was defined.
+2. A cross-sectoral objective for the OH surveillance system was defined but is not based on stakeholders’ expectations.
+3. A cross-sectoral objective for the OH surveillance system was defined based on some stakeholders’ expectations.
+4. A cross-sectoral objective for the OH surveillance system was defined based on all stakeholders’ expectations.</t>
   </si>
 </sst>
 </file>
@@ -1874,44 +1873,44 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="97.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" customWidth="1"/>
+    <col min="2" max="2" width="97.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="24.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="7" width="21.7265625" customWidth="1"/>
     <col min="8" max="8" width="27" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.1796875" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="23.85546875" customWidth="1"/>
+    <col min="12" max="12" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:281" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:281" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
     </row>
-    <row r="2" spans="1:281" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:281" ht="92.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
       <c r="D2" s="33"/>
     </row>
-    <row r="3" spans="1:281" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:281" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>4</v>
@@ -2194,133 +2193,133 @@
       <c r="JT3" s="5"/>
       <c r="JU3" s="5"/>
     </row>
-    <row r="4" spans="1:281" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:281" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="34" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
       <c r="D4" s="35"/>
     </row>
-    <row r="5" spans="1:281" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:281" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:281" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B6" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:281" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:281" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="C6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="7" spans="1:281" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+    <row r="8" spans="1:281" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B8" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="8" spans="1:281" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="C8" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="9" spans="1:281" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:281" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
       <c r="B9" s="19"/>
     </row>
-    <row r="10" spans="1:281" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:281" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" t="s">
+        <v>240</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:281" ht="87" x14ac:dyDescent="0.35">
+      <c r="A11" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B11" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:281" x14ac:dyDescent="0.35">
+      <c r="A12" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="C12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:281" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="C13" t="s">
         <v>241</v>
       </c>
-      <c r="D10" s="20" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="11" spans="1:281" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="C11" t="s">
-        <v>241</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="12" spans="1:281" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="B12" s="20" t="s">
+      <c r="D13" s="29" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:281" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="C12" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="13" spans="1:281" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>242</v>
       </c>
-      <c r="D13" s="29" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="14" spans="1:281" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="D14" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="B14" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="C14" t="s">
-        <v>243</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="15" spans="1:281" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:281" x14ac:dyDescent="0.35">
       <c r="A15" s="18"/>
     </row>
-    <row r="16" spans="1:281" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:281" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
     </row>
   </sheetData>
@@ -2340,22 +2339,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:JU23"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="89.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="39.54296875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="89.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="105" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="5" customWidth="1"/>
-    <col min="6" max="281" width="9.140625" style="5"/>
-    <col min="282" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="8.26953125" style="5" customWidth="1"/>
+    <col min="6" max="281" width="9.1796875" style="5"/>
+    <col min="282" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:281" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:281" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -2640,9 +2639,9 @@
       <c r="JT1" s="5"/>
       <c r="JU1" s="5"/>
     </row>
-    <row r="2" spans="1:281" s="2" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:281" s="2" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
@@ -2925,7 +2924,7 @@
       <c r="JT2" s="5"/>
       <c r="JU2" s="5"/>
     </row>
-    <row r="3" spans="1:281" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:281" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>2</v>
@@ -3214,7 +3213,7 @@
       <c r="JT3" s="5"/>
       <c r="JU3" s="5"/>
     </row>
-    <row r="4" spans="1:281" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:281" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="39" t="s">
         <v>1</v>
       </c>
@@ -3499,7 +3498,7 @@
       <c r="JT4" s="5"/>
       <c r="JU4" s="5"/>
     </row>
-    <row r="5" spans="1:281" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:281" s="4" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
@@ -3510,7 +3509,7 @@
         <v>45</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>46</v>
+        <v>244</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3790,7 +3789,7 @@
       <c r="JT5" s="5"/>
       <c r="JU5" s="5"/>
     </row>
-    <row r="6" spans="1:281" ht="183" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:281" ht="183" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
@@ -3798,13 +3797,13 @@
         <v>17</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:281" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:281" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
@@ -3812,10 +3811,10 @@
         <v>18</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -4095,7 +4094,7 @@
       <c r="JT7" s="5"/>
       <c r="JU7" s="5"/>
     </row>
-    <row r="8" spans="1:281" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:281" ht="212.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>26</v>
       </c>
@@ -4103,13 +4102,13 @@
         <v>19</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:281" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:281" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="39" t="s">
         <v>5</v>
       </c>
@@ -4394,7 +4393,7 @@
       <c r="JT9" s="5"/>
       <c r="JU9" s="5"/>
     </row>
-    <row r="10" spans="1:281" s="4" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:281" s="4" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>27</v>
       </c>
@@ -4402,10 +4401,10 @@
         <v>43</v>
       </c>
       <c r="C10" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -4685,7 +4684,7 @@
       <c r="JT10" s="5"/>
       <c r="JU10" s="5"/>
     </row>
-    <row r="11" spans="1:281" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:281" ht="122.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>28</v>
       </c>
@@ -4693,24 +4692,24 @@
         <v>42</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:281" s="4" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:281" s="4" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="D12" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>59</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -4990,7 +4989,7 @@
       <c r="JT12" s="5"/>
       <c r="JU12" s="5"/>
     </row>
-    <row r="13" spans="1:281" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:281" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>30</v>
       </c>
@@ -4998,13 +4997,13 @@
         <v>41</v>
       </c>
       <c r="C13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:281" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:281" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="39" t="s">
         <v>6</v>
       </c>
@@ -5289,7 +5288,7 @@
       <c r="JT14" s="5"/>
       <c r="JU14" s="5"/>
     </row>
-    <row r="15" spans="1:281" s="4" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:281" s="4" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>31</v>
       </c>
@@ -5297,10 +5296,10 @@
         <v>20</v>
       </c>
       <c r="C15" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>62</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>63</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -5580,7 +5579,7 @@
       <c r="JT15" s="5"/>
       <c r="JU15" s="5"/>
     </row>
-    <row r="16" spans="1:281" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:281" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>32</v>
       </c>
@@ -5588,24 +5587,24 @@
         <v>21</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:281" s="4" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:281" s="4" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="D17" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -5885,7 +5884,7 @@
       <c r="JT17" s="5"/>
       <c r="JU17" s="5"/>
     </row>
-    <row r="18" spans="1:281" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:281" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>34</v>
       </c>
@@ -5893,13 +5892,13 @@
         <v>22</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:281" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:281" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="39" t="s">
         <v>7</v>
       </c>
@@ -6184,18 +6183,18 @@
       <c r="JT19" s="5"/>
       <c r="JU19" s="5"/>
     </row>
-    <row r="20" spans="1:281" s="4" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:281" s="4" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="D20" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -6475,21 +6474,21 @@
       <c r="JT20" s="5"/>
       <c r="JU20" s="5"/>
     </row>
-    <row r="21" spans="1:281" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:281" ht="110.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:281" s="4" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:281" s="4" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>37</v>
       </c>
@@ -6497,10 +6496,10 @@
         <v>40</v>
       </c>
       <c r="C22" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>78</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -6780,7 +6779,7 @@
       <c r="JT22" s="5"/>
       <c r="JU22" s="5"/>
     </row>
-    <row r="23" spans="1:281" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:281" ht="150" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>38</v>
       </c>
@@ -6788,10 +6787,10 @@
         <v>39</v>
       </c>
       <c r="C23" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -6813,19 +6812,19 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:D19"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" style="7" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="85.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="85.26953125" style="7" customWidth="1"/>
     <col min="4" max="4" width="114" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="7"/>
+    <col min="5" max="16384" width="9.1796875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="46" t="s">
         <v>8</v>
       </c>
@@ -6833,15 +6832,15 @@
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
     </row>
-    <row r="2" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="48"/>
       <c r="C2" s="48"/>
       <c r="D2" s="49"/>
     </row>
-    <row r="3" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>2</v>
@@ -6853,7 +6852,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="43" t="s">
         <v>9</v>
       </c>
@@ -6861,63 +6860,63 @@
       <c r="C4" s="44"/>
       <c r="D4" s="45"/>
     </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="8" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="8" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" s="12" t="s">
+      <c r="B6" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="8" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="8" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" s="8" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="8" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="8" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>112</v>
-      </c>
       <c r="C8" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="43" t="s">
         <v>10</v>
       </c>
@@ -6925,63 +6924,63 @@
       <c r="C9" s="44"/>
       <c r="D9" s="45"/>
     </row>
-    <row r="10" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="C11" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D11" s="15" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="12" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="15" t="s">
+      <c r="C12" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D12" s="12" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+    <row r="13" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="C13" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D13" s="15" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="43" t="s">
         <v>11</v>
       </c>
@@ -6989,63 +6988,63 @@
       <c r="C14" s="44"/>
       <c r="D14" s="45"/>
     </row>
-    <row r="15" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D16" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+    <row r="17" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" s="12" t="s">
+      <c r="C17" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D17" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+    <row r="18" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="15" t="s">
+      <c r="C18" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D18" s="12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="43" t="s">
         <v>12</v>
       </c>
@@ -7053,60 +7052,60 @@
       <c r="C19" s="44"/>
       <c r="D19" s="45"/>
     </row>
-    <row r="20" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="D21" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="D22" s="14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+    <row r="23" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D23" s="12" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -7128,20 +7127,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="73.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="105.140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="73.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="105.1796875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="53" t="s">
         <v>13</v>
       </c>
@@ -7149,15 +7148,15 @@
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
     </row>
-    <row r="2" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="52" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" s="52"/>
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
     </row>
-    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="24"/>
       <c r="B3" s="24" t="s">
         <v>2</v>
@@ -7169,7 +7168,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="51" t="s">
         <v>14</v>
       </c>
@@ -7177,65 +7176,65 @@
       <c r="C4" s="51"/>
       <c r="D4" s="51"/>
     </row>
-    <row r="5" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="26" t="s">
+      <c r="B6" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D6" s="23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+    <row r="7" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B7" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C7" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D7" s="26" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>183</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="51" t="s">
         <v>15</v>
       </c>
@@ -7243,63 +7242,63 @@
       <c r="C9" s="51"/>
       <c r="D9" s="51"/>
     </row>
-    <row r="10" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="C10" s="26" t="s">
+      <c r="B11" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D11" s="23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+    <row r="12" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="C11" s="23" t="s">
+      <c r="B12" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D12" s="26" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+    <row r="13" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="B12" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="C12" s="26" t="s">
+      <c r="B13" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D13" s="23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="51" t="s">
         <v>16</v>
       </c>
@@ -7307,124 +7306,124 @@
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
     </row>
-    <row r="15" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B16" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C16" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D16" s="23" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+    <row r="17" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B17" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="C16" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="D16" s="23" t="s">
+      <c r="C18" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="D18" s="23" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="51" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
       <c r="D19" s="51"/>
     </row>
-    <row r="20" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="B20" s="25" t="s">
-        <v>222</v>
-      </c>
-      <c r="C20" s="26" t="s">
+      <c r="B21" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D21" s="23" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+    <row r="22" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="B21" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="C21" s="27" t="s">
+      <c r="B22" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D22" s="26" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+    <row r="23" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="B22" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="C22" s="26" t="s">
+      <c r="B23" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="C23" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D23" s="23" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverted questionnaire , as some trouble with extra spaces and character vs numeric formating of indicator IDs
</commit_message>
<xml_diff>
--- a/data/EU-EpiCap_Questionnaire_21_11_30.xlsx
+++ b/data/EU-EpiCap_Questionnaire_21_11_30.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://surreyac-my.sharepoint.com/personal/cb0078_surrey_ac_uk/Documents/MATRIX/WP4-T2/EU-EpiCap-Tool/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{45270A84-C129-4EA0-9102-B014D4D5961B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{28526098-AC66-4E22-BDF6-508079EF737A}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="8_{B2ED66EE-9066-4F67-9A9C-C5FF33F2DB6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{23D3E7C1-36B1-4C96-B703-ECB05BA3AD8E}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="1050" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="5" r:id="rId1"/>
@@ -342,13 +342,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1. There has never been an internal evaluation of the functioning of the OH surveillance system.
-2. Internal evaluations of the functioning of the system have been conducted but only punctually. The set of indicators is insufficient and could be substantially improved.
-3. Internal evaluations of the functioning of the system have been conducted but they remain irregular or the set of indicators could be improved to enable a better monitoring of the functioning of the OH surveillance system. 
-4. Internal evaluations of the functioning of the system have been conducted regularly, using an exhaustive system of relevant indicators.
-</t>
-  </si>
-  <si>
     <t>External evaluation of the OH surveillance system</t>
   </si>
   <si>
@@ -394,9 +387,6 @@
     <t>2.13</t>
   </si>
   <si>
-    <t xml:space="preserve">2.14 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Data sharing agreement</t>
   </si>
   <si>
@@ -410,9 +400,6 @@
   </si>
   <si>
     <t xml:space="preserve">Usefulness of shared data </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.23 </t>
   </si>
   <si>
     <t xml:space="preserve"> FAIR data (Data management plan, Interoperability, storage and accessibility).</t>
@@ -475,11 +462,6 @@
   </si>
   <si>
     <t>Collaborative design of surveillance protocols</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.11 How would you consider the collaborative efforts across sectors to design surveillance protocols?
-List of collaborators, activities, outputs, strength and weakness of the collaboration to design surveillance protocols are defined (including financial, human and material resources).
-</t>
   </si>
   <si>
     <t xml:space="preserve">NA. The surveillance system does not require surveillance protocol.
@@ -1112,6 +1094,23 @@
   </si>
   <si>
     <t>Target 3.4 Ultimate outcomes</t>
+  </si>
+  <si>
+    <t>2.14</t>
+  </si>
+  <si>
+    <t>1. There has never been an internal evaluation of the functioning of the OH surveillance system.
+2. Internal evaluations of the functioning of the system have been conducted but only punctually. The set of indicators is insufficient and could be substantially improved.
+3. Internal evaluations of the functioning of the system have been conducted but they remain irregular or the set of indicators could be improved to enable a better monitoring of the functioning of the OH surveillance system. 
+4. Internal evaluations of the functioning of the system have been conducted regularly, using an exhaustive system of relevant indicators.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How would you consider the collaborative efforts across sectors to design surveillance protocols?
+List of collaborators, activities, outputs, strength and weakness of the collaboration to design surveillance protocols are defined (including financial, human and material resources).
+</t>
+  </si>
+  <si>
+    <t>2.23</t>
   </si>
   <si>
     <t>1. No cross-sectoral objective was defined.
@@ -1359,7 +1358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1445,6 +1444,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1873,44 +1890,44 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.54296875" customWidth="1"/>
-    <col min="2" max="2" width="97.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
-    <col min="4" max="4" width="24.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="97.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
     <col min="8" max="8" width="27" customWidth="1"/>
-    <col min="9" max="9" width="17.1796875" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="23.81640625" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:281" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
-        <v>207</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-    </row>
-    <row r="2" spans="1:281" ht="92.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="32" t="s">
-        <v>219</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-    </row>
-    <row r="3" spans="1:281" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:281" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+    </row>
+    <row r="2" spans="1:281" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+    </row>
+    <row r="3" spans="1:281" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>4</v>
@@ -2193,133 +2210,133 @@
       <c r="JT3" s="5"/>
       <c r="JU3" s="5"/>
     </row>
-    <row r="4" spans="1:281" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
+    <row r="4" spans="1:281" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+    </row>
+    <row r="5" spans="1:281" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:281" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:281" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="C7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:281" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-    </row>
-    <row r="5" spans="1:281" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="C5" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="6" spans="1:281" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="C6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="7" spans="1:281" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="C7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:281" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>212</v>
-      </c>
       <c r="C8" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="9" spans="1:281" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:281" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="19"/>
     </row>
-    <row r="10" spans="1:281" ht="87" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:281" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="C10" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:281" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="C11" t="s">
+        <v>236</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:281" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="C12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:281" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="C10" t="s">
-        <v>240</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="11" spans="1:281" ht="87" x14ac:dyDescent="0.35">
-      <c r="A11" s="28" t="s">
+      <c r="B13" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" t="s">
+        <v>237</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:281" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="C11" t="s">
-        <v>240</v>
-      </c>
-      <c r="D11" s="20" t="s">
+      <c r="B14" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:281" x14ac:dyDescent="0.35">
-      <c r="A12" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="C12" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="13" spans="1:281" ht="58" x14ac:dyDescent="0.35">
-      <c r="A13" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="C13" t="s">
-        <v>241</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:281" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>216</v>
-      </c>
-      <c r="C14" t="s">
-        <v>242</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="15" spans="1:281" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:281" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
     </row>
-    <row r="16" spans="1:281" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:281" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
   </sheetData>
@@ -2339,28 +2356,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:JU23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="39.54296875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="89.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="89.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="105" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" style="5" customWidth="1"/>
-    <col min="6" max="281" width="9.1796875" style="5"/>
-    <col min="282" max="16384" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="8.28515625" style="5" customWidth="1"/>
+    <col min="6" max="281" width="9.140625" style="5"/>
+    <col min="282" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:281" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:281" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -2639,13 +2656,13 @@
       <c r="JT1" s="5"/>
       <c r="JU1" s="5"/>
     </row>
-    <row r="2" spans="1:281" s="2" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
+    <row r="2" spans="1:281" s="2" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -2924,7 +2941,7 @@
       <c r="JT2" s="5"/>
       <c r="JU2" s="5"/>
     </row>
-    <row r="3" spans="1:281" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:281" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>2</v>
@@ -3213,13 +3230,13 @@
       <c r="JT3" s="5"/>
       <c r="JU3" s="5"/>
     </row>
-    <row r="4" spans="1:281" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="39" t="s">
+    <row r="4" spans="1:281" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -3498,7 +3515,7 @@
       <c r="JT4" s="5"/>
       <c r="JU4" s="5"/>
     </row>
-    <row r="5" spans="1:281" s="4" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:281" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
@@ -3789,7 +3806,7 @@
       <c r="JT5" s="5"/>
       <c r="JU5" s="5"/>
     </row>
-    <row r="6" spans="1:281" ht="183" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:281" ht="183" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
@@ -3803,7 +3820,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:281" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:281" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
@@ -4094,7 +4111,7 @@
       <c r="JT7" s="5"/>
       <c r="JU7" s="5"/>
     </row>
-    <row r="8" spans="1:281" ht="212.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:281" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>26</v>
       </c>
@@ -4108,13 +4125,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:281" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="39" t="s">
+    <row r="9" spans="1:281" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="47"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -4393,7 +4410,7 @@
       <c r="JT9" s="5"/>
       <c r="JU9" s="5"/>
     </row>
-    <row r="10" spans="1:281" s="4" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:281" s="4" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>27</v>
       </c>
@@ -4684,7 +4701,7 @@
       <c r="JT10" s="5"/>
       <c r="JU10" s="5"/>
     </row>
-    <row r="11" spans="1:281" ht="122.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:281" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>28</v>
       </c>
@@ -4698,7 +4715,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:281" s="4" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:281" s="4" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>29</v>
       </c>
@@ -4989,7 +5006,7 @@
       <c r="JT12" s="5"/>
       <c r="JU12" s="5"/>
     </row>
-    <row r="13" spans="1:281" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:281" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>30</v>
       </c>
@@ -5003,13 +5020,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:281" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="39" t="s">
+    <row r="14" spans="1:281" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="41"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -5288,7 +5305,7 @@
       <c r="JT14" s="5"/>
       <c r="JU14" s="5"/>
     </row>
-    <row r="15" spans="1:281" s="4" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:281" s="4" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>31</v>
       </c>
@@ -5579,7 +5596,7 @@
       <c r="JT15" s="5"/>
       <c r="JU15" s="5"/>
     </row>
-    <row r="16" spans="1:281" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:281" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>32</v>
       </c>
@@ -5593,7 +5610,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:281" s="4" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:281" s="4" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>33</v>
       </c>
@@ -5884,7 +5901,7 @@
       <c r="JT17" s="5"/>
       <c r="JU17" s="5"/>
     </row>
-    <row r="18" spans="1:281" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:281" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>34</v>
       </c>
@@ -5898,13 +5915,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:281" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="39" t="s">
+    <row r="19" spans="1:281" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="47"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -6183,7 +6200,7 @@
       <c r="JT19" s="5"/>
       <c r="JU19" s="5"/>
     </row>
-    <row r="20" spans="1:281" s="4" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:281" s="4" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>35</v>
       </c>
@@ -6194,7 +6211,7 @@
         <v>71</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>72</v>
+        <v>241</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -6474,21 +6491,21 @@
       <c r="JT20" s="5"/>
       <c r="JU20" s="5"/>
     </row>
-    <row r="21" spans="1:281" ht="110.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:281" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:281" s="4" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:281" s="4" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>37</v>
       </c>
@@ -6496,10 +6513,10 @@
         <v>40</v>
       </c>
       <c r="C22" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>76</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>77</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -6779,7 +6796,7 @@
       <c r="JT22" s="5"/>
       <c r="JU22" s="5"/>
     </row>
-    <row r="23" spans="1:281" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:281" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>38</v>
       </c>
@@ -6787,10 +6804,10 @@
         <v>39</v>
       </c>
       <c r="C23" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -6811,37 +6828,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="7" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="85.26953125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="35" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="85.28515625" style="7" customWidth="1"/>
     <col min="4" max="4" width="114" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="7"/>
+    <col min="5" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-    </row>
-    <row r="2" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="49"/>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+    </row>
+    <row r="2" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="55"/>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
       <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
@@ -6852,260 +6869,260 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="43" t="s">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
-    </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
+    </row>
+    <row r="5" spans="1:4" s="8" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="8" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B6" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="D6" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="8" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="8" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="15" t="s">
+      <c r="D7" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="8" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="51"/>
+    </row>
+    <row r="10" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="8" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="D11" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" s="8" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="45"/>
-    </row>
-    <row r="10" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="D12" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="51"/>
+    </row>
+    <row r="15" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="D15" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="D16" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13" s="15" t="s">
+      <c r="D17" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="45"/>
-    </row>
-    <row r="15" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="D15" s="15" t="s">
+      <c r="D18" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+    </row>
+    <row r="20" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D16" s="12" t="s">
+      <c r="C20" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="D21" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="45"/>
-    </row>
-    <row r="20" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="13" t="s">
+      <c r="D22" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="12" t="s">
+      <c r="D23" s="12" t="s">
         <v>137</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -7128,35 +7145,35 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A3" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="73.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="105.1796875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="5.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="73.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="105.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-    </row>
-    <row r="2" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-    </row>
-    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+    </row>
+    <row r="2" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="24" t="s">
         <v>2</v>
@@ -7168,262 +7185,262 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="51" t="s">
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-    </row>
-    <row r="5" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+    </row>
+    <row r="5" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="24" t="s">
+      <c r="C6" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>151</v>
-      </c>
       <c r="C7" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>178</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>182</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+    </row>
+    <row r="10" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="C10" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="D8" s="23" t="s">
+      <c r="B12" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-    </row>
-    <row r="10" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="D10" s="26" t="s">
+      <c r="D13" s="23" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+    </row>
+    <row r="15" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="26" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="B11" s="24" t="s">
+      <c r="D15" s="26" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D13" s="23" t="s">
+      <c r="B18" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="23" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-    </row>
-    <row r="15" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="25" t="s">
+      <c r="D18" s="23" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="57" t="s">
+        <v>239</v>
+      </c>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+    </row>
+    <row r="20" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="D15" s="26" t="s">
+      <c r="B20" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" s="27" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="D16" s="23" t="s">
+      <c r="D21" s="23" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" s="26" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="24" t="s">
+      <c r="D22" s="26" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="D18" s="23" t="s">
+      <c r="B23" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="23" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-    </row>
-    <row r="20" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>200</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="C23" s="23" t="s">
+      <c r="D23" s="23" t="s">
         <v>202</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>